<commit_message>
many images from phone of assembly
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MEMSduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4159DBDD-E834-49CB-926C-04B1FADEA627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F37F9E-1556-4726-B05B-7C5A18F4C287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1860" windowWidth="26865" windowHeight="12735" xr2:uid="{964DCA75-9C03-4665-A5C3-D212B2818574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>description</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>number in order</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>hardware</t>
+  </si>
+  <si>
+    <t>vendor part number</t>
+  </si>
+  <si>
+    <t>manufacturer part number</t>
   </si>
 </sst>
 </file>
@@ -414,50 +426,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9227DDD-8365-4864-A5FB-3571E7A7DE36}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="1" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improving structure of documentation
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MEMSduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1363B46-77B1-4846-9363-C0FEDBE6BAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9A14D4-189E-433E-B66A-FC2BC8F732BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="3300" windowWidth="20910" windowHeight="13980" xr2:uid="{964DCA75-9C03-4665-A5C3-D212B2818574}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{964DCA75-9C03-4665-A5C3-D212B2818574}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="132">
   <si>
     <t>description</t>
   </si>
@@ -351,6 +351,87 @@
   </si>
   <si>
     <t>custom printed circuit board</t>
+  </si>
+  <si>
+    <t>PCBWay</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/DROK-Boost-Converter-Regulator-Length/dp/B09M3LMSS3/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Voltage-Converter-Vintage-Indicator-80V-380V/dp/B09D93QNYK</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/dfrobot/DFR0216/6579366</t>
+  </si>
+  <si>
+    <t>DFR0216</t>
+  </si>
+  <si>
+    <t>DFRobot</t>
+  </si>
+  <si>
+    <t>1738-1228-ND</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/assmann-wsw-components/AK672-2-2/947492</t>
+  </si>
+  <si>
+    <t>Assmann</t>
+  </si>
+  <si>
+    <t>1835-1117-ND</t>
+  </si>
+  <si>
+    <t>Comus International</t>
+  </si>
+  <si>
+    <t>3570-1331-053</t>
+  </si>
+  <si>
+    <t>AE1493-ND</t>
+  </si>
+  <si>
+    <t>AK672/2-2</t>
+  </si>
+  <si>
+    <t>https://github.com/lafefspietz/MEMSduino/blob/main/3dprint_files/arduino-bracket.STL</t>
+  </si>
+  <si>
+    <t>https://github.com/lafefspietz/MEMSduino/blob/main/3dprint_files/HV-DCDC-bracket.STL</t>
+  </si>
+  <si>
+    <t>https://github.com/lafefspietz/MEMSduino/blob/main/3dprint_files/front-panel-center-bracket.STL</t>
+  </si>
+  <si>
+    <t>https://github.com/lafefspietz/MEMSduino/blob/main/3dprint_files/front-panel-edge-bracket.STL</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/ZYAMY-Dupont-Connector-Multicolor-Breadboard/dp/B0B8Z23NWX/</t>
+  </si>
+  <si>
+    <t>https://aivon.fi</t>
+  </si>
+  <si>
+    <t>3dJake</t>
+  </si>
+  <si>
+    <t>ruthex</t>
+  </si>
+  <si>
+    <t>RUT-GE-4-40x57-001</t>
+  </si>
+  <si>
+    <t>GE-4-40x57-001</t>
+  </si>
+  <si>
+    <t>machined brass</t>
+  </si>
+  <si>
+    <t>H Bracket</t>
   </si>
 </sst>
 </file>
@@ -745,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9227DDD-8365-4864-A5FB-3571E7A7DE36}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +900,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" ref="G2:G19" si="0">$E2*$F2</f>
+        <f t="shared" ref="G2:G20" si="0">$E2*$F2</f>
         <v>6.96</v>
       </c>
       <c r="H2" t="s">
@@ -1093,7 +1174,16 @@
         <v>0.51100000000000001</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>126</v>
+      </c>
+      <c r="I11" t="s">
+        <v>128</v>
+      </c>
+      <c r="J11" t="s">
+        <v>127</v>
+      </c>
+      <c r="K11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1337,8 +1427,33 @@
       <c r="B20" s="3" t="s">
         <v>96</v>
       </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>70</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.43</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>28.599999999999998</v>
+      </c>
+      <c r="H20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" t="s">
+        <v>115</v>
+      </c>
+      <c r="J20" t="s">
+        <v>116</v>
+      </c>
+      <c r="K20" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1364,6 +1479,18 @@
         <f>$E21*$F21</f>
         <v>11.25</v>
       </c>
+      <c r="H21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21">
+        <v>1559</v>
+      </c>
+      <c r="J21" t="s">
+        <v>112</v>
+      </c>
+      <c r="K21">
+        <v>1559</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1375,6 +1502,31 @@
       <c r="C22" t="s">
         <v>98</v>
       </c>
+      <c r="D22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="2">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <f>$E22*$F22</f>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="H22" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" t="s">
+        <v>111</v>
+      </c>
+      <c r="J22" t="s">
+        <v>110</v>
+      </c>
+      <c r="K22" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1386,6 +1538,19 @@
       <c r="C23" t="s">
         <v>98</v>
       </c>
+      <c r="D23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <f>$E23*$F23</f>
+        <v>7.99</v>
+      </c>
       <c r="H23" t="s">
         <v>83</v>
       </c>
@@ -1400,6 +1565,19 @@
       <c r="C24" t="s">
         <v>98</v>
       </c>
+      <c r="D24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="2">
+        <v>11.39</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <f>$E24*$F24</f>
+        <v>11.39</v>
+      </c>
       <c r="H24" t="s">
         <v>83</v>
       </c>
@@ -1414,6 +1592,31 @@
       <c r="C25" t="s">
         <v>99</v>
       </c>
+      <c r="D25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2">
+        <f>$E25*$F25</f>
+        <v>1.64</v>
+      </c>
+      <c r="H25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" t="s">
+        <v>118</v>
+      </c>
+      <c r="J25" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1425,6 +1628,19 @@
       <c r="C26" t="s">
         <v>100</v>
       </c>
+      <c r="D26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
+        <f>$E26*$F26</f>
+        <v>5.99</v>
+      </c>
       <c r="H26" t="s">
         <v>83</v>
       </c>
@@ -1439,6 +1655,9 @@
       <c r="C27" t="s">
         <v>100</v>
       </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
       <c r="H27" t="s">
         <v>83</v>
       </c>
@@ -1453,6 +1672,9 @@
       <c r="C28" t="s">
         <v>100</v>
       </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
       <c r="H28" t="s">
         <v>83</v>
       </c>
@@ -1467,6 +1689,9 @@
       <c r="C29" t="s">
         <v>78</v>
       </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
       <c r="G29" s="2">
         <f>$E29*$F29</f>
         <v>0</v>
@@ -1482,6 +1707,15 @@
       <c r="C30" t="s">
         <v>104</v>
       </c>
+      <c r="E30" s="2">
+        <v>5.98</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1493,6 +1727,15 @@
       <c r="C31" t="s">
         <v>104</v>
       </c>
+      <c r="E31" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1504,8 +1747,17 @@
       <c r="C32" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -1515,8 +1767,17 @@
       <c r="C33" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -1526,8 +1787,14 @@
       <c r="C34" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -1537,8 +1804,14 @@
       <c r="C35" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -1548,8 +1821,14 @@
       <c r="C36" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -1559,10 +1838,63 @@
       <c r="C37" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>93</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1588,8 +1920,18 @@
     <hyperlink ref="D18" r:id="rId18" xr:uid="{902A0660-9FAE-4FA1-959B-93D22B2DD4BA}"/>
     <hyperlink ref="D15" r:id="rId19" xr:uid="{9B1C1D5D-2C03-47AA-BB33-8431974A2977}"/>
     <hyperlink ref="D19" r:id="rId20" xr:uid="{00FFBDFA-D5D6-4F77-94B2-779A1D711FDC}"/>
+    <hyperlink ref="D23" r:id="rId21" xr:uid="{A0A966D5-1F40-4F33-8226-1F0A965C797B}"/>
+    <hyperlink ref="D24" r:id="rId22" xr:uid="{6BE55BDB-8E4D-4B62-8F37-9315C26C127A}"/>
+    <hyperlink ref="D22" r:id="rId23" xr:uid="{EFBF539C-618E-43E0-A62F-575BF38DD6A9}"/>
+    <hyperlink ref="D25" r:id="rId24" xr:uid="{F1A68759-4C17-495E-AF4C-35EBB710BB0C}"/>
+    <hyperlink ref="D34" r:id="rId25" xr:uid="{15E103AF-EAB5-4FDF-A5EE-5BBEEE5FC290}"/>
+    <hyperlink ref="D35" r:id="rId26" xr:uid="{D03C1B69-4D48-4795-9E93-BE0E22931B25}"/>
+    <hyperlink ref="D36" r:id="rId27" xr:uid="{549C9F63-3406-4568-9EB9-2E3F9A8F50D2}"/>
+    <hyperlink ref="D37" r:id="rId28" xr:uid="{8CE89076-BF96-48E9-8823-7820AD88138C}"/>
+    <hyperlink ref="D26" r:id="rId29" xr:uid="{884619D7-502D-401A-901D-2363033DC363}"/>
+    <hyperlink ref="D38" r:id="rId30" xr:uid="{3ECC4416-4EC7-4521-89D4-53BB9BC8F581}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId21"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
custom metal box docs
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MEMSduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59C829F-2D35-41B8-9835-38D6D28905A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1819427-FC3E-4C85-90D8-C1AA3439B954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{964DCA75-9C03-4665-A5C3-D212B2818574}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{964DCA75-9C03-4665-A5C3-D212B2818574}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -849,25 +849,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9227DDD-8365-4864-A5FB-3571E7A7DE36}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="67.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="58.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="67.453125" customWidth="1"/>
+    <col min="2" max="2" width="30.81640625" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" customWidth="1"/>
+    <col min="4" max="4" width="58.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.7265625" customWidth="1"/>
+    <col min="10" max="10" width="28.453125" customWidth="1"/>
+    <col min="11" max="11" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -902,7 +902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -932,7 +932,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -962,7 +962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -992,7 +992,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>93</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>130</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>131</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>132</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>133</v>
       </c>

</xml_diff>

<commit_message>
tons of documentation work
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MEMSduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1819427-FC3E-4C85-90D8-C1AA3439B954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25C31A1-5D0E-4037-9390-7F2985A428A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{964DCA75-9C03-4665-A5C3-D212B2818574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="139">
   <si>
     <t>description</t>
   </si>
@@ -185,9 +185,6 @@
     <t>0.1" headers</t>
   </si>
   <si>
-    <t>Neopixel</t>
-  </si>
-  <si>
     <t>Arduino UNO</t>
   </si>
   <si>
@@ -449,10 +446,13 @@
     <t>https://www.amazon.com/ZYAMY-Dupont-Connector-Multicolor-Breadboard/dp/B0789F523N/</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/amphenol-cs-commercial-products/G800W268018EU/17083164</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.amazon.com/ZYAMY-Dupont-Connector-Multicolor-Breadboard/dp/B0789F2Y1T/ </t>
+  </si>
+  <si>
+    <t>Neopixel programmable RGB LED</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Header-Lystaii-Pin-Connector-Electronic/dp/B06ZZN8L9S/</t>
   </si>
 </sst>
 </file>
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9227DDD-8365-4864-A5FB-3571E7A7DE36}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1144,16 +1144,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="2">
         <v>1.62</v>
@@ -1169,21 +1169,21 @@
         <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11">
         <v>7.2999999999999995E-2</v>
@@ -1196,16 +1196,16 @@
         <v>0.51100000000000001</v>
       </c>
       <c r="H11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J11" t="s">
         <v>125</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>127</v>
-      </c>
-      <c r="J11" t="s">
-        <v>126</v>
-      </c>
-      <c r="K11" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -1213,13 +1213,13 @@
         <v>41</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="2">
         <v>0.1</v>
@@ -1232,7 +1232,7 @@
         <v>0.1</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -1240,13 +1240,13 @@
         <v>42</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2">
         <v>0.05</v>
@@ -1259,7 +1259,7 @@
         <v>0.45</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1267,13 +1267,13 @@
         <v>43</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="2">
         <v>0.1</v>
@@ -1286,7 +1286,7 @@
         <v>0.2</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1294,13 +1294,13 @@
         <v>44</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" s="2">
         <v>0.51</v>
@@ -1313,7 +1313,7 @@
         <v>0.51</v>
       </c>
       <c r="H15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1321,13 +1321,13 @@
         <v>45</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="2">
         <v>0.28999999999999998</v>
@@ -1340,21 +1340,21 @@
         <v>2.61</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" s="2">
         <v>3.7999999999999999E-2</v>
@@ -1367,7 +1367,7 @@
         <v>0.76</v>
       </c>
       <c r="H17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1375,13 +1375,13 @@
         <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E18" s="2">
         <v>1.17</v>
@@ -1394,16 +1394,16 @@
         <v>1.17</v>
       </c>
       <c r="H18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I18" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" t="s">
         <v>80</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>81</v>
-      </c>
-      <c r="K18" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1411,13 +1411,13 @@
         <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E19" s="2">
         <v>61.3</v>
@@ -1430,30 +1430,30 @@
         <v>61.3</v>
       </c>
       <c r="H19" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" t="s">
+        <v>75</v>
+      </c>
+      <c r="J19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K19" t="s">
         <v>73</v>
-      </c>
-      <c r="I19" t="s">
-        <v>76</v>
-      </c>
-      <c r="J19" t="s">
-        <v>75</v>
-      </c>
-      <c r="K19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="2">
         <v>1.43</v>
@@ -1466,30 +1466,30 @@
         <v>28.599999999999998</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I20" t="s">
+        <v>113</v>
+      </c>
+      <c r="J20" t="s">
         <v>114</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>115</v>
-      </c>
-      <c r="K20" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2">
         <v>1.25</v>
@@ -1498,17 +1498,17 @@
         <v>9</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" ref="G21:G26" si="1">$E21*$F21</f>
+        <f t="shared" ref="G21:G28" si="1">$E21*$F21</f>
         <v>11.25</v>
       </c>
       <c r="H21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I21">
         <v>1559</v>
       </c>
       <c r="J21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K21">
         <v>1559</v>
@@ -1516,16 +1516,16 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" s="2">
         <v>16.899999999999999</v>
@@ -1538,30 +1538,30 @@
         <v>16.899999999999999</v>
       </c>
       <c r="H22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E23" s="2">
         <v>7.99</v>
@@ -1574,21 +1574,21 @@
         <v>7.99</v>
       </c>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E24" s="2">
         <v>11.39</v>
@@ -1601,21 +1601,21 @@
         <v>11.39</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E25" s="2">
         <v>1.64</v>
@@ -1628,83 +1628,97 @@
         <v>1.64</v>
       </c>
       <c r="H25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I25" t="s">
+        <v>116</v>
+      </c>
+      <c r="J25" t="s">
+        <v>80</v>
+      </c>
+      <c r="K25" t="s">
         <v>117</v>
-      </c>
-      <c r="J25" t="s">
-        <v>81</v>
-      </c>
-      <c r="K25" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E26" s="2">
-        <v>5.99</v>
+        <v>0.59899999999999998</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" si="1"/>
-        <v>5.99</v>
+        <v>0.59899999999999998</v>
       </c>
       <c r="H26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.79</v>
       </c>
       <c r="F27">
         <v>9</v>
       </c>
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>7.11</v>
+      </c>
       <c r="H27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.99</v>
       </c>
       <c r="F28">
         <v>2</v>
       </c>
+      <c r="G28" s="2">
+        <f t="shared" si="1"/>
+        <v>1.98</v>
+      </c>
       <c r="H28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -1712,31 +1726,37 @@
         <v>48</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.09</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G29" s="2">
         <f>$E29*$F29</f>
-        <v>0</v>
+        <v>0.27</v>
+      </c>
+      <c r="H29" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E30" s="2">
         <v>5.98</v>
@@ -1745,18 +1765,18 @@
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" s="2">
         <v>1.82</v>
@@ -1765,18 +1785,18 @@
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E32" s="2">
         <v>1.82</v>
@@ -1785,18 +1805,18 @@
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E33" s="2">
         <v>1.4</v>
@@ -1805,175 +1825,175 @@
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F36">
         <v>2</v>
       </c>
       <c r="H36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F37">
         <v>2</v>
       </c>
       <c r="H37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F38">
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2010,10 +2030,9 @@
     <hyperlink ref="D26" r:id="rId29" xr:uid="{884619D7-502D-401A-901D-2363033DC363}"/>
     <hyperlink ref="D38" r:id="rId30" xr:uid="{3ECC4416-4EC7-4521-89D4-53BB9BC8F581}"/>
     <hyperlink ref="D27" r:id="rId31" xr:uid="{F448C947-6DA4-41EF-9F1C-DF0DACBB4455}"/>
-    <hyperlink ref="D29" r:id="rId32" xr:uid="{09E99870-FE0C-4948-97ED-B3432299E939}"/>
-    <hyperlink ref="D28" r:id="rId33" display="https://www.amazon.com/ZYAMY-Dupont-Connector-Multicolor-Breadboard/dp/B0789F2Y1T/" xr:uid="{874914B1-8AFA-4BDC-8AC4-C9395C0DB705}"/>
+    <hyperlink ref="D28" r:id="rId32" display="https://www.amazon.com/ZYAMY-Dupont-Connector-Multicolor-Breadboard/dp/B0789F2Y1T/" xr:uid="{874914B1-8AFA-4BDC-8AC4-C9395C0DB705}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId34"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved the sp6t layout template, readme flow, bom
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MEMSduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25C31A1-5D0E-4037-9390-7F2985A428A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EFC46B6-F168-4296-B7A8-465C75EAC6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{964DCA75-9C03-4665-A5C3-D212B2818574}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{964DCA75-9C03-4665-A5C3-D212B2818574}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -520,7 +520,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -531,6 +531,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -847,27 +848,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9227DDD-8365-4864-A5FB-3571E7A7DE36}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.453125" customWidth="1"/>
-    <col min="2" max="2" width="30.81640625" customWidth="1"/>
-    <col min="3" max="3" width="29.453125" customWidth="1"/>
-    <col min="4" max="4" width="58.54296875" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="67.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="23.7265625" customWidth="1"/>
-    <col min="10" max="10" width="28.453125" customWidth="1"/>
-    <col min="11" max="11" width="26.1796875" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -902,7 +903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -932,7 +933,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -962,7 +963,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -992,7 +993,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1022,7 +1023,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1052,7 +1053,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1082,7 +1083,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1172,7 +1173,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1235,7 +1236,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1262,7 +1263,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1289,7 +1290,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1316,7 +1317,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1406,7 +1407,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -1514,7 +1515,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1550,7 +1551,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1577,7 +1578,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1640,7 +1641,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1667,7 +1668,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1694,7 +1695,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1721,7 +1722,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -1748,7 +1749,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>83</v>
       </c>
@@ -1764,11 +1765,15 @@
       <c r="F30">
         <v>1</v>
       </c>
+      <c r="G30" s="2">
+        <f t="shared" ref="G30:G33" si="2">$E30*$F30</f>
+        <v>5.98</v>
+      </c>
       <c r="H30" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -1784,11 +1789,15 @@
       <c r="F31">
         <v>1</v>
       </c>
+      <c r="G31" s="2">
+        <f t="shared" si="2"/>
+        <v>1.82</v>
+      </c>
       <c r="H31" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -1804,11 +1813,15 @@
       <c r="F32">
         <v>1</v>
       </c>
+      <c r="G32" s="2">
+        <f t="shared" si="2"/>
+        <v>1.82</v>
+      </c>
       <c r="H32" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -1824,11 +1837,15 @@
       <c r="F33">
         <v>1</v>
       </c>
+      <c r="G33" s="2">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
       <c r="H33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -1848,7 +1865,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>88</v>
       </c>
@@ -1868,7 +1885,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -1888,7 +1905,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>90</v>
       </c>
@@ -1908,7 +1925,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>92</v>
       </c>
@@ -1928,7 +1945,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>129</v>
       </c>
@@ -1945,7 +1962,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>130</v>
       </c>
@@ -1962,7 +1979,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>131</v>
       </c>
@@ -1979,7 +1996,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>132</v>
       </c>
@@ -1994,6 +2011,12 @@
       </c>
       <c r="H42" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G44" s="6">
+        <f>SUM(G2:G43)</f>
+        <v>218.13799999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>